<commit_message>
fix bug for channel zztestzz
</commit_message>
<xml_diff>
--- a/test_upload_short/temp_upload.xlsx
+++ b/test_upload_short/temp_upload.xlsx
@@ -425,7 +425,7 @@
     <outlinePr summaryBelow="1" summaryRight="1"/>
     <pageSetUpPr/>
   </sheetPr>
-  <dimension ref="A1:H2"/>
+  <dimension ref="A1:H3"/>
   <sheetViews>
     <sheetView workbookViewId="0">
       <selection activeCell="A1" sqref="A1"/>
@@ -518,6 +518,48 @@
         </is>
       </c>
     </row>
+    <row r="3">
+      <c r="A3" t="inlineStr">
+        <is>
+          <t>"\\192.168.1.92\Ổ Sever Mới\Định\Satisfy ASMR\New folder\45s - MUSIC\Tuấn\Amazing Slime\UP\406 number A.mp4"</t>
+        </is>
+      </c>
+      <c r="B3" t="inlineStr">
+        <is>
+          <t>zzTESTzz</t>
+        </is>
+      </c>
+      <c r="C3" t="inlineStr">
+        <is>
+          <t>The king of the pirates</t>
+        </is>
+      </c>
+      <c r="D3" t="inlineStr">
+        <is>
+          <t>To make holding a key convenient, the hold() function can be used as a context manager and passed a string from the pyautogui.KEYBOARD_KEYS such as shift, ctrl, alt, and this key will be held for the duration of the with context block. See KEYBOARD_KEYS.</t>
+        </is>
+      </c>
+      <c r="E3" t="inlineStr">
+        <is>
+          <t>15:31</t>
+        </is>
+      </c>
+      <c r="F3" t="inlineStr">
+        <is>
+          <t>11/9/2026</t>
+        </is>
+      </c>
+      <c r="G3" t="inlineStr">
+        <is>
+          <t>Uploaded</t>
+        </is>
+      </c>
+      <c r="H3" t="inlineStr">
+        <is>
+          <t>https://youtube.com/shorts/1q90a0XStHA</t>
+        </is>
+      </c>
+    </row>
   </sheetData>
   <pageMargins left="0.75" right="0.75" top="1" bottom="1" header="0.5" footer="0.5"/>
 </worksheet>

</xml_diff>

<commit_message>
fixxing csv data and code
</commit_message>
<xml_diff>
--- a/test_upload_short/temp_upload.xlsx
+++ b/test_upload_short/temp_upload.xlsx
@@ -526,7 +526,7 @@
       </c>
       <c r="B3" t="inlineStr">
         <is>
-          <t>zzTESTzz</t>
+          <t>Mushroom Toy Unboxing</t>
         </is>
       </c>
       <c r="C3" t="inlineStr">
@@ -556,7 +556,7 @@
       </c>
       <c r="H3" t="inlineStr">
         <is>
-          <t>https://youtube.com/shorts/1q90a0XStHA</t>
+          <t>https://youtube.com/shorts/GN4ZrQ95wO8</t>
         </is>
       </c>
     </row>

</xml_diff>

<commit_message>
fixing update sheet  and up too fast
</commit_message>
<xml_diff>
--- a/test_upload_short/temp_upload.xlsx
+++ b/test_upload_short/temp_upload.xlsx
@@ -425,7 +425,7 @@
     <outlinePr summaryBelow="1" summaryRight="1"/>
     <pageSetUpPr/>
   </sheetPr>
-  <dimension ref="A1:G11"/>
+  <dimension ref="A1:G23"/>
   <sheetViews>
     <sheetView workbookViewId="0">
       <selection activeCell="A1" sqref="A1"/>
@@ -583,7 +583,7 @@
       </c>
       <c r="G4" t="inlineStr">
         <is>
-          <t>Upload</t>
+          <t>Uploaded</t>
         </is>
       </c>
     </row>
@@ -856,7 +856,502 @@
       <c r="D11" t="inlineStr"/>
       <c r="E11" t="inlineStr"/>
       <c r="F11" t="inlineStr"/>
-      <c r="G11" t="inlineStr"/>
+      <c r="G11" t="inlineStr">
+        <is>
+          <t>Uploaded</t>
+        </is>
+      </c>
+    </row>
+    <row r="12">
+      <c r="A12" t="inlineStr">
+        <is>
+          <t>"\\192.168.1.92\Ổ Sever Mới\Định\Satisfy ASMR\New folder\45s - MUSIC\Tuấn\Slime Squishing\152BA.mp4"</t>
+        </is>
+      </c>
+      <c r="B12" t="inlineStr">
+        <is>
+          <t>Slime Squishing</t>
+        </is>
+      </c>
+      <c r="C12" t="inlineStr">
+        <is>
+          <t>💘 ASMR Slime Squishing so Satisfying Relaxing #SlimeSquishing #slimeasmr #asmrslime #satisfying</t>
+        </is>
+      </c>
+      <c r="D12" t="inlineStr">
+        <is>
+          <t>🍡💘 ASMR Slime Squishing so Satisfying Nutella 🍩
+#SlimeSquishing #Slime #ASMR #Satisfying #Shorts #YouTubeShorts
+#pipingbags  #slimeasmr #asmrslime 
+slime asmr, asmr slime, satisfying
+Thank you for watching the video. Please subscribe to Slime Squishing to watch our latest videos! Wish you have relaxing moments with Slime Squishing.</t>
+        </is>
+      </c>
+      <c r="E12" t="inlineStr">
+        <is>
+          <t>22:00</t>
+        </is>
+      </c>
+      <c r="F12" t="inlineStr">
+        <is>
+          <t>11/9/2026</t>
+        </is>
+      </c>
+      <c r="G12" t="inlineStr">
+        <is>
+          <t>Uploaded</t>
+        </is>
+      </c>
+    </row>
+    <row r="13">
+      <c r="A13" t="inlineStr">
+        <is>
+          <t>"\\192.168.1.92\Ổ Sever Mới\Định\Satisfy ASMR\New folder\45s - MUSIC\Tuấn\Slime Squishing\154BA.mp4"</t>
+        </is>
+      </c>
+      <c r="B13" t="inlineStr">
+        <is>
+          <t>Slime Squishing</t>
+        </is>
+      </c>
+      <c r="C13" t="inlineStr">
+        <is>
+          <t>❤️🧡💛💚💙💜 ASMR Slime Squishing 💝 so Satisfying #SlimeSquishing #slimeasmr #asmrslime #satisfying</t>
+        </is>
+      </c>
+      <c r="D13" t="inlineStr">
+        <is>
+          <t>❤️🧡💛💚💙💜 ASMR Slime Squishing 💝 so Satisfying
+#SlimeSquishing #Slime #ASMR #Satisfying #Shorts #YouTubeShorts
+#pipingbags  #slimeasmr #asmrslime 
+slime asmr, asmr slime, satisfying
+Thank you for watching the video. Please subscribe to Slime Squishing to watch our latest videos! Wish you have relaxing moments with Slime Squishing.</t>
+        </is>
+      </c>
+      <c r="E13" t="inlineStr">
+        <is>
+          <t>2:00</t>
+        </is>
+      </c>
+      <c r="F13" t="inlineStr">
+        <is>
+          <t>12/9/2025</t>
+        </is>
+      </c>
+      <c r="G13" t="inlineStr">
+        <is>
+          <t>Uploaded</t>
+        </is>
+      </c>
+    </row>
+    <row r="14">
+      <c r="A14" t="inlineStr">
+        <is>
+          <t>"\\192.168.1.92\Ổ Sever Mới\Định\Satisfy ASMR\New folder\45s - MUSIC\Tuấn\Slime Squishing\156BA.mp4"</t>
+        </is>
+      </c>
+      <c r="B14" t="inlineStr">
+        <is>
+          <t>Slime Squishing</t>
+        </is>
+      </c>
+      <c r="C14" t="inlineStr">
+        <is>
+          <t>🍡💘 ASMR Slime Squishing so Satisfying Relaxing #SlimeSquishing #slimeasmr #asmrslime #satisfying</t>
+        </is>
+      </c>
+      <c r="D14" t="inlineStr">
+        <is>
+          <t>🍡💘 ASMR Slime Squishing so Satisfying Nutella 🍩
+#SlimeSquishing #Slime #ASMR #Satisfying #Shorts #YouTubeShorts
+#pipingbags  #slimeasmr #asmrslime 
+slime asmr, asmr slime, satisfying
+Thank you for watching the video. Please subscribe to Slime Squishing to watch our latest videos! Wish you have relaxing moments with Slime Squishing.</t>
+        </is>
+      </c>
+      <c r="E14" t="inlineStr">
+        <is>
+          <t>10:00</t>
+        </is>
+      </c>
+      <c r="F14" t="inlineStr">
+        <is>
+          <t>12/9/2025</t>
+        </is>
+      </c>
+      <c r="G14" t="inlineStr">
+        <is>
+          <t>Uploaded</t>
+        </is>
+      </c>
+    </row>
+    <row r="15">
+      <c r="A15" t="inlineStr">
+        <is>
+          <t>"\\192.168.1.92\Ổ Sever Mới\Định\Satisfy ASMR\New folder\45s - MUSIC\Tuấn\Slime Squishing\158BA.mp4"</t>
+        </is>
+      </c>
+      <c r="B15" t="inlineStr">
+        <is>
+          <t>Slime Squishing</t>
+        </is>
+      </c>
+      <c r="C15" t="inlineStr">
+        <is>
+          <t>💦 Topping slime 🧼 dried floam 💥 mixing ASMR  #SlimeSquishing #slimeasmr #asmrslime #satisfying</t>
+        </is>
+      </c>
+      <c r="D15" t="inlineStr">
+        <is>
+          <t>💦 Topping slime 🧼 dried floam 💥 mixing ASMR
+#SlimeSquishing #Slime #ASMR #Satisfying #Shorts #YouTubeShorts
+#pipingbags  #slimeasmr #asmrslime 
+slime asmr, asmr slime, satisfying
+Thank you for watching the video. Please subscribe to Slime Squishing to watch our latest videos! Wish you have relaxing moments with Slime Squishing.</t>
+        </is>
+      </c>
+      <c r="E15" t="inlineStr">
+        <is>
+          <t>22:00</t>
+        </is>
+      </c>
+      <c r="F15" t="inlineStr">
+        <is>
+          <t>12/9/2025</t>
+        </is>
+      </c>
+      <c r="G15" t="inlineStr">
+        <is>
+          <t>Uploaded</t>
+        </is>
+      </c>
+    </row>
+    <row r="16">
+      <c r="A16" t="inlineStr">
+        <is>
+          <t>"\\192.168.1.92\Ổ Sever Mới\Định\Satisfy ASMR\New folder\45s - MUSIC\Tuấn\Slime Squishing\160BA.mp4"</t>
+        </is>
+      </c>
+      <c r="B16" t="inlineStr">
+        <is>
+          <t>Slime Squishing</t>
+        </is>
+      </c>
+      <c r="C16" t="inlineStr">
+        <is>
+          <t>❤️🧡💛💚💙💜 ASMR Slime Squishing 💝 so Satisfying #SlimeSquishing #slimeasmr #asmrslime #satisfying</t>
+        </is>
+      </c>
+      <c r="D16" t="inlineStr">
+        <is>
+          <t>❤️🧡💛💚💙💜 ASMR Slime Squishing 💝 so Satisfying
+#SlimeSquishing #Slime #ASMR #Satisfying #Shorts #YouTubeShorts
+#pipingbags  #slimeasmr #asmrslime 
+slime asmr, asmr slime, satisfying
+Thank you for watching the video. Please subscribe to Slime Squishing to watch our latest videos! Wish you have relaxing moments with Slime Squishing.</t>
+        </is>
+      </c>
+      <c r="E16" t="inlineStr">
+        <is>
+          <t>2:00</t>
+        </is>
+      </c>
+      <c r="F16" t="inlineStr">
+        <is>
+          <t>13/9/2025</t>
+        </is>
+      </c>
+      <c r="G16" t="inlineStr">
+        <is>
+          <t>Uploaded</t>
+        </is>
+      </c>
+    </row>
+    <row r="17">
+      <c r="A17" t="inlineStr">
+        <is>
+          <t>"\\192.168.1.92\Ổ Sever Mới\Định\Satisfy ASMR\New folder\45s - MUSIC\Tuấn\Slime Squishing\162BA.mp4"</t>
+        </is>
+      </c>
+      <c r="B17" t="inlineStr">
+        <is>
+          <t>Slime Squishing</t>
+        </is>
+      </c>
+      <c r="C17" t="inlineStr">
+        <is>
+          <t>🤩 ASMR Slime Squishing so Satisfying Relaxing #SlimeSquishing #slimeasmr #asmrslime #satisfying</t>
+        </is>
+      </c>
+      <c r="D17" t="inlineStr">
+        <is>
+          <t>🤩 ASMR Slime Squishing so Satisfying
+#SlimeSquishing #Slime #ASMR #Satisfying #Shorts #YouTubeShorts
+#pipingbags  #slimeasmr #asmrslime 
+slime asmr, asmr slime, satisfying
+Thank you for watching the video. Please subscribe to Slime Squishing to watch our latest videos! Wish you have relaxing moments with Slime Squishing.</t>
+        </is>
+      </c>
+      <c r="E17" t="inlineStr">
+        <is>
+          <t>10:00</t>
+        </is>
+      </c>
+      <c r="F17" t="inlineStr">
+        <is>
+          <t>13/9/2025</t>
+        </is>
+      </c>
+      <c r="G17" t="inlineStr">
+        <is>
+          <t>Uploaded</t>
+        </is>
+      </c>
+    </row>
+    <row r="18">
+      <c r="A18" t="inlineStr">
+        <is>
+          <t>"\\192.168.1.92\Ổ Sever Mới\Định\Satisfy ASMR\New folder\45s - MUSIC\Tuấn\Relaxing Squishy\130AA.mp4"</t>
+        </is>
+      </c>
+      <c r="B18" t="inlineStr">
+        <is>
+          <t>Relaxing SquishySquishy</t>
+        </is>
+      </c>
+      <c r="C18" t="inlineStr">
+        <is>
+          <t>🍎🎈 Relaxing Squishy #bubblesound #stressballasmr #crunchystressballasmr #bubbleasmr</t>
+        </is>
+      </c>
+      <c r="D18" t="inlineStr">
+        <is>
+          <t>#RelaxingSquishy #asmr #satisfying #relaxing #mixing #relax #stressrelief #bubblesound #stressballasmr #squishytungtungsahur #crunchystressballasmr #bubbleasmr
+bubble sound, stress ball asmr, squishy tung tung sahur, crunchy stress ball asmr, bubble asmr
+💬 What did you think of the video?
+👇 Drop your thoughts in the comments below!
+👍 If you enjoyed it, don’t forget to give it a like
+🔔 Subscribe and turn on the bell so you never miss a new upload!
+📢 Share this video with your friends too!
+Thanks for watching and supporting Relaxing Squishy! 💖</t>
+        </is>
+      </c>
+      <c r="E18" t="inlineStr">
+        <is>
+          <t>21:00</t>
+        </is>
+      </c>
+      <c r="F18" t="inlineStr">
+        <is>
+          <t>11/9/2025</t>
+        </is>
+      </c>
+      <c r="G18" t="inlineStr"/>
+    </row>
+    <row r="19">
+      <c r="A19" t="inlineStr">
+        <is>
+          <t>"\\192.168.1.92\Ổ Sever Mới\Định\Satisfy ASMR\New folder\45s - MUSIC\Tuấn\Relaxing Squishy\132AA.mp4"</t>
+        </is>
+      </c>
+      <c r="B19" t="inlineStr">
+        <is>
+          <t>Relaxing SquishySquishy</t>
+        </is>
+      </c>
+      <c r="C19" t="inlineStr">
+        <is>
+          <t xml:space="preserve">💥👉 Relaxing Squishy #bubblesound #stressballasmr #crunchystressballasmr #bubbleasmr
+</t>
+        </is>
+      </c>
+      <c r="D19" t="inlineStr">
+        <is>
+          <t>#RelaxingSquishy #asmr #satisfying #relaxing #mixing #relax #stressrelief #bubblesound #stressballasmr #squishytungtungsahur #crunchystressballasmr #bubbleasmr
+bubble sound, stress ball asmr, squishy tung tung sahur, crunchy stress ball asmr, bubble asmr
+💬 What did you think of the video?
+👇 Drop your thoughts in the comments below!
+👍 If you enjoyed it, don’t forget to give it a like
+🔔 Subscribe and turn on the bell so you never miss a new upload!
+📢 Share this video with your friends too!
+Thanks for watching and supporting Relaxing Squishy! 💖</t>
+        </is>
+      </c>
+      <c r="E19" t="inlineStr">
+        <is>
+          <t>1:00</t>
+        </is>
+      </c>
+      <c r="F19" t="inlineStr">
+        <is>
+          <t>12/9/2025</t>
+        </is>
+      </c>
+      <c r="G19" t="inlineStr"/>
+    </row>
+    <row r="20">
+      <c r="A20" t="inlineStr">
+        <is>
+          <t>"\\192.168.1.92\Ổ Sever Mới\Định\Satisfy ASMR\New folder\45s - MUSIC\Tuấn\Relaxing Squishy\134AA.mp4"</t>
+        </is>
+      </c>
+      <c r="B20" t="inlineStr">
+        <is>
+          <t>Relaxing SquishySquishy</t>
+        </is>
+      </c>
+      <c r="C20" t="inlineStr">
+        <is>
+          <t xml:space="preserve">🎉👉 Relaxing Squishy #bubblesound #stressballasmr #crunchystressballasmr #bubbleasmr
+</t>
+        </is>
+      </c>
+      <c r="D20" t="inlineStr">
+        <is>
+          <t>#RelaxingSquishy #asmr #satisfying #relaxing #mixing #relax #stressrelief #bubblesound #stressballasmr #squishytungtungsahur #crunchystressballasmr #bubbleasmr
+bubble sound, stress ball asmr, squishy tung tung sahur, crunchy stress ball asmr, bubble asmr
+💬 What did you think of the video?
+👇 Drop your thoughts in the comments below!
+👍 If you enjoyed it, don’t forget to give it a like
+🔔 Subscribe and turn on the bell so you never miss a new upload!
+📢 Share this video with your friends too!
+Thanks for watching and supporting Relaxing Squishy! 💖</t>
+        </is>
+      </c>
+      <c r="E20" t="inlineStr">
+        <is>
+          <t>9:00</t>
+        </is>
+      </c>
+      <c r="F20" t="inlineStr">
+        <is>
+          <t>12/9/2025</t>
+        </is>
+      </c>
+      <c r="G20" t="inlineStr"/>
+    </row>
+    <row r="21">
+      <c r="A21" t="inlineStr">
+        <is>
+          <t>"\\192.168.1.92\Ổ Sever Mới\Định\Satisfy ASMR\New folder\45s - MUSIC\Tuấn\Relaxing Squishy\136AA.mp4"</t>
+        </is>
+      </c>
+      <c r="B21" t="inlineStr">
+        <is>
+          <t>Relaxing SquishySquishy</t>
+        </is>
+      </c>
+      <c r="C21" t="inlineStr">
+        <is>
+          <t xml:space="preserve">💦🧁 Relaxing Squishy #bubblesound #stressballasmr #crunchystressballasmr #bubbleasmr
+</t>
+        </is>
+      </c>
+      <c r="D21" t="inlineStr">
+        <is>
+          <t>#RelaxingSquishy #asmr #satisfying #relaxing #mixing #relax #stressrelief #bubblesound #stressballasmr #squishytungtungsahur #crunchystressballasmr #bubbleasmr
+bubble sound, stress ball asmr, squishy tung tung sahur, crunchy stress ball asmr, bubble asmr
+💬 What did you think of the video?
+👇 Drop your thoughts in the comments below!
+👍 If you enjoyed it, don’t forget to give it a like
+🔔 Subscribe and turn on the bell so you never miss a new upload!
+📢 Share this video with your friends too!
+Thanks for watching and supporting Relaxing Squishy! 💖</t>
+        </is>
+      </c>
+      <c r="E21" t="inlineStr">
+        <is>
+          <t>21:00</t>
+        </is>
+      </c>
+      <c r="F21" t="inlineStr">
+        <is>
+          <t>12/9/2025</t>
+        </is>
+      </c>
+      <c r="G21" t="inlineStr"/>
+    </row>
+    <row r="22">
+      <c r="A22" t="inlineStr">
+        <is>
+          <t>"\\192.168.1.92\Ổ Sever Mới\Định\Satisfy ASMR\New folder\45s - MUSIC\Tuấn\Relaxing Squishy\138AA.mp4"</t>
+        </is>
+      </c>
+      <c r="B22" t="inlineStr">
+        <is>
+          <t>Relaxing SquishySquishy</t>
+        </is>
+      </c>
+      <c r="C22" t="inlineStr">
+        <is>
+          <t xml:space="preserve">👀 Relaxing Squishy #bubblesound #stressballasmr #crunchystressballasmr #bubbleasmr
+</t>
+        </is>
+      </c>
+      <c r="D22" t="inlineStr">
+        <is>
+          <t>#RelaxingSquishy #asmr #satisfying #relaxing #mixing #relax #stressrelief #bubblesound #stressballasmr #squishytungtungsahur #crunchystressballasmr #bubbleasmr
+bubble sound, stress ball asmr, squishy tung tung sahur, crunchy stress ball asmr, bubble asmr
+💬 What did you think of the video?
+👇 Drop your thoughts in the comments below!
+👍 If you enjoyed it, don’t forget to give it a like
+🔔 Subscribe and turn on the bell so you never miss a new upload!
+📢 Share this video with your friends too!
+Thanks for watching and supporting Relaxing Squishy! 💖</t>
+        </is>
+      </c>
+      <c r="E22" t="inlineStr">
+        <is>
+          <t>1:00</t>
+        </is>
+      </c>
+      <c r="F22" t="inlineStr">
+        <is>
+          <t>13/9/2025</t>
+        </is>
+      </c>
+      <c r="G22" t="inlineStr"/>
+    </row>
+    <row r="23">
+      <c r="A23" t="inlineStr">
+        <is>
+          <t>"\\192.168.1.92\Ổ Sever Mới\Định\Satisfy ASMR\New folder\45s - MUSIC\Tuấn\Relaxing Squishy\140AA.mp4"</t>
+        </is>
+      </c>
+      <c r="B23" t="inlineStr">
+        <is>
+          <t>Relaxing SquishySquishy</t>
+        </is>
+      </c>
+      <c r="C23" t="inlineStr">
+        <is>
+          <t xml:space="preserve">💞💕 Relaxing Squishy #bubblesound #stressballasmr #crunchystressballasmr #bubbleasmr
+</t>
+        </is>
+      </c>
+      <c r="D23" t="inlineStr">
+        <is>
+          <t>#RelaxingSquishy #asmr #satisfying #relaxing #mixing #relax #stressrelief #bubblesound #stressballasmr #squishytungtungsahur #crunchystressballasmr #bubbleasmr
+bubble sound, stress ball asmr, squishy tung tung sahur, crunchy stress ball asmr, bubble asmr
+💬 What did you think of the video?
+👇 Drop your thoughts in the comments below!
+👍 If you enjoyed it, don’t forget to give it a like
+🔔 Subscribe and turn on the bell so you never miss a new upload!
+📢 Share this video with your friends too!
+Thanks for watching and supporting Relaxing Squishy! 💖</t>
+        </is>
+      </c>
+      <c r="E23" t="inlineStr">
+        <is>
+          <t>9:00</t>
+        </is>
+      </c>
+      <c r="F23" t="inlineStr">
+        <is>
+          <t>13/9/2025</t>
+        </is>
+      </c>
+      <c r="G23" t="inlineStr"/>
     </row>
   </sheetData>
   <pageMargins left="0.75" right="0.75" top="1" bottom="1" header="0.5" footer="0.5"/>

</xml_diff>

<commit_message>
remove url and playlist part
</commit_message>
<xml_diff>
--- a/test_upload_short/temp_upload.xlsx
+++ b/test_upload_short/temp_upload.xlsx
@@ -425,7 +425,7 @@
     <outlinePr summaryBelow="1" summaryRight="1"/>
     <pageSetUpPr/>
   </sheetPr>
-  <dimension ref="A1:H11"/>
+  <dimension ref="A1:G11"/>
   <sheetViews>
     <sheetView workbookViewId="0">
       <selection activeCell="A1" sqref="A1"/>
@@ -469,11 +469,6 @@
           <t>status</t>
         </is>
       </c>
-      <c r="H1" s="1" t="inlineStr">
-        <is>
-          <t>URL</t>
-        </is>
-      </c>
     </row>
     <row r="2">
       <c r="A2" t="inlineStr">
@@ -512,11 +507,6 @@
           <t>Uploaded</t>
         </is>
       </c>
-      <c r="H2" t="inlineStr">
-        <is>
-          <t>https://youtube.com/shorts/qaZbXUZT7zo</t>
-        </is>
-      </c>
     </row>
     <row r="3">
       <c r="A3" t="inlineStr">
@@ -554,11 +544,6 @@
           <t>Uploaded</t>
         </is>
       </c>
-      <c r="H3" t="inlineStr">
-        <is>
-          <t>https://youtube.com/shorts/GN4ZrQ95wO8</t>
-        </is>
-      </c>
     </row>
     <row r="4">
       <c r="A4" t="inlineStr">
@@ -573,7 +558,7 @@
       </c>
       <c r="C4" t="inlineStr">
         <is>
-          <t>⚡🌟 Miniature food &amp; fruits ASMR Sound Review 🤯 #cooker #cookingtoys #ricecooker #kitchentoys</t>
+          <t>test video</t>
         </is>
       </c>
       <c r="D4" t="inlineStr">
@@ -598,12 +583,7 @@
       </c>
       <c r="G4" t="inlineStr">
         <is>
-          <t>Failed</t>
-        </is>
-      </c>
-      <c r="H4" t="inlineStr">
-        <is>
-          <t>18:00</t>
+          <t>Upload</t>
         </is>
       </c>
     </row>
@@ -648,11 +628,6 @@
           <t>Failed</t>
         </is>
       </c>
-      <c r="H5" t="inlineStr">
-        <is>
-          <t>22:00</t>
-        </is>
-      </c>
     </row>
     <row r="6">
       <c r="A6" t="inlineStr">
@@ -695,11 +670,6 @@
           <t>Failed</t>
         </is>
       </c>
-      <c r="H6" t="inlineStr">
-        <is>
-          <t>2:00</t>
-        </is>
-      </c>
     </row>
     <row r="7">
       <c r="A7" t="inlineStr">
@@ -742,11 +712,6 @@
           <t>Failed</t>
         </is>
       </c>
-      <c r="H7" t="inlineStr">
-        <is>
-          <t>18:00</t>
-        </is>
-      </c>
     </row>
     <row r="8">
       <c r="A8" t="inlineStr">
@@ -789,11 +754,6 @@
           <t>Failed</t>
         </is>
       </c>
-      <c r="H8" t="inlineStr">
-        <is>
-          <t>22:00</t>
-        </is>
-      </c>
     </row>
     <row r="9">
       <c r="A9" t="inlineStr">
@@ -834,11 +794,6 @@
       <c r="G9" t="inlineStr">
         <is>
           <t>Failed</t>
-        </is>
-      </c>
-      <c r="H9" t="inlineStr">
-        <is>
-          <t>2:00</t>
         </is>
       </c>
     </row>
@@ -885,11 +840,6 @@
           <t>Failed</t>
         </is>
       </c>
-      <c r="H10" t="inlineStr">
-        <is>
-          <t>18:30</t>
-        </is>
-      </c>
     </row>
     <row r="11">
       <c r="A11" t="inlineStr">
@@ -897,13 +847,16 @@
           <t>"\\192.168.1.92\Ổ Sever Mới\Định\Satisfy ASMR\New folder\Short Toy\Natra\Hoàn thiện\260AC.mp4"</t>
         </is>
       </c>
-      <c r="B11" t="inlineStr"/>
+      <c r="B11" t="inlineStr">
+        <is>
+          <t>Mushroom Toy Unboxing</t>
+        </is>
+      </c>
       <c r="C11" t="inlineStr"/>
       <c r="D11" t="inlineStr"/>
       <c r="E11" t="inlineStr"/>
       <c r="F11" t="inlineStr"/>
       <c r="G11" t="inlineStr"/>
-      <c r="H11" t="inlineStr"/>
     </row>
   </sheetData>
   <pageMargins left="0.75" right="0.75" top="1" bottom="1" header="0.5" footer="0.5"/>

</xml_diff>